<commit_message>
Todays Changes To Flows and Control Relationships
</commit_message>
<xml_diff>
--- a/ky_fpr/Development/Documents/Design/InterviewCascade.xlsx
+++ b/ky_fpr/Development/Documents/Design/InterviewCascade.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>MRE</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Add Investigation</t>
+  </si>
+  <si>
+    <t>What if NMR is NOT PC ?</t>
+  </si>
+  <si>
+    <t>What if BPTW is NOT PC ?</t>
   </si>
 </sst>
 </file>
@@ -490,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -502,14 +508,15 @@
     <col min="4" max="4" width="24.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" customWidth="1"/>
     <col min="7" max="7" width="17.09765625" customWidth="1"/>
+    <col min="8" max="8" width="27.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>8</v>
       </c>
@@ -523,7 +530,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -534,7 +541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -544,8 +551,11 @@
       <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -559,7 +569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -567,7 +577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>1</v>
       </c>
@@ -577,13 +587,16 @@
       <c r="G8" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>6</v>
       </c>
@@ -594,7 +607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>6</v>
       </c>
@@ -605,7 +618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>2</v>
       </c>
@@ -616,7 +629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
COB stable FPR for quit and discharge
</commit_message>
<xml_diff>
--- a/ky_fpr/Development/Documents/Design/InterviewCascade.xlsx
+++ b/ky_fpr/Development/Documents/Design/InterviewCascade.xlsx
@@ -114,10 +114,10 @@
     <t>Add Investigation</t>
   </si>
   <si>
-    <t>What if NMR is NOT PC ?</t>
-  </si>
-  <si>
-    <t>What if BPTW is NOT PC ?</t>
+    <t>Even if BPTW is NOT PC</t>
+  </si>
+  <si>
+    <t>Even if NMR is NOT PC</t>
   </si>
 </sst>
 </file>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -552,7 +552,7 @@
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -588,7 +588,7 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Separation Interview Selection Changes
</commit_message>
<xml_diff>
--- a/ky_fpr/Development/Documents/Design/InterviewCascade.xlsx
+++ b/ky_fpr/Development/Documents/Design/InterviewCascade.xlsx
@@ -64,7 +64,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Recen Concurrent with MRE Employment</t>
+Recent Concurrent with MRE Employment</t>
         </r>
       </text>
     </comment>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
   <si>
     <t>MRE</t>
   </si>
@@ -84,9 +84,6 @@
     <t>BPTW</t>
   </si>
   <si>
-    <t>10W</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -118,13 +115,21 @@
   </si>
   <si>
     <t>Even if NMR is NOT PC</t>
+  </si>
+  <si>
+    <t>Employment 
+10W</t>
+  </si>
+  <si>
+    <t>Employer 
+10W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -149,6 +154,20 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -189,12 +208,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,36 +524,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.69921875" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" customWidth="1"/>
+    <col min="2" max="2" width="2.09765625" customWidth="1"/>
+    <col min="3" max="3" width="5.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="12.296875" customWidth="1"/>
     <col min="7" max="7" width="17.09765625" customWidth="1"/>
     <col min="8" max="8" width="27.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -535,10 +565,10 @@
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -546,13 +576,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -574,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -582,40 +612,45 @@
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
         <v>6</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="F12" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -623,10 +658,10 @@
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -634,13 +669,14 @@
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>